<commit_message>
Check the time for CUDA. It's mainly on MALLOC CUDA_HISTOGRAM_PTR!!!
</commit_message>
<xml_diff>
--- a/Evaluation/speedup table.xlsx
+++ b/Evaluation/speedup table.xlsx
@@ -44,10 +44,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Communication time in train</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>test time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -61,6 +57,10 @@
   </si>
   <si>
     <t>correct rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initCUDA time in train</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,7 +389,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -405,13 +405,13 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>9.6142000000000005E-2</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.122294</v>

</xml_diff>

<commit_message>
Update the result of openmpi on the index = 0 dataset
</commit_message>
<xml_diff>
--- a/Evaluation/speedup table.xlsx
+++ b/Evaluation/speedup table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Sequential</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,10 @@
   </si>
   <si>
     <t>initCUDA time in train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>communication time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -386,15 +390,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -405,16 +412,19 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -427,14 +437,14 @@
       <c r="D2">
         <v>2.4949999999999998E-3</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.19014800000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.75407000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -447,14 +457,14 @@
       <c r="D3">
         <v>2.918E-3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.231462</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.75407000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -467,19 +477,37 @@
       <c r="D4">
         <v>1.5200000000000001E-3</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.210538</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.75946499999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
+      <c r="B5">
+        <v>0.15035599999999999</v>
+      </c>
+      <c r="C5">
+        <v>7.4898999999999993E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.7390000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>1.7E-5</v>
+      </c>
+      <c r="G5">
+        <v>0.199686</v>
+      </c>
+      <c r="H5">
+        <v>0.75407000000000002</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -492,13 +520,13 @@
       <c r="D6">
         <v>1.0095E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.178782</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.14721899999999999</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.75946499999999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the result of speedup table. Update the problems of evaluation into final report.md
</commit_message>
<xml_diff>
--- a/Evaluation/speedup table.xlsx
+++ b/Evaluation/speedup table.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="a1a" sheetId="1" r:id="rId1"/>
+    <sheet name="ijcnn1" sheetId="2" r:id="rId2"/>
+    <sheet name="generated" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>Sequential</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,6 +67,10 @@
   </si>
   <si>
     <t>communication time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,000011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -392,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -535,4 +541,266 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.5315059999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.8905190000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.28919299999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.54247800000000002</v>
+      </c>
+      <c r="H2">
+        <v>0.67373300000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2.4280279999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.563461</v>
+      </c>
+      <c r="D3">
+        <v>0.53073899999999996</v>
+      </c>
+      <c r="G3">
+        <v>0.65548200000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.67373300000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>17.892775</v>
+      </c>
+      <c r="C5">
+        <v>6.2186599999999999</v>
+      </c>
+      <c r="D5">
+        <v>22.483117</v>
+      </c>
+      <c r="E5">
+        <v>1.1E-5</v>
+      </c>
+      <c r="H5">
+        <v>0.95622700000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3.6024859999999999</v>
+      </c>
+      <c r="C6">
+        <v>3.1373679999999999</v>
+      </c>
+      <c r="D6">
+        <v>8.6230000000000005E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.113554</v>
+      </c>
+      <c r="G6">
+        <v>0.44085099999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.90499600000000002</v>
+      </c>
+    </row>
+    <row r="22" ht="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>20.206942000000002</v>
+      </c>
+      <c r="C2">
+        <v>13.738770000000001</v>
+      </c>
+      <c r="D2">
+        <v>4.6531690000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.44645600000000002</v>
+      </c>
+      <c r="H2">
+        <v>0.59909999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>13.650181</v>
+      </c>
+      <c r="C3">
+        <v>6.5865970000000003</v>
+      </c>
+      <c r="D3">
+        <v>5.2281789999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.47265299999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.59909999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>203.485626</v>
+      </c>
+      <c r="C5">
+        <v>40.328243999999998</v>
+      </c>
+      <c r="D5">
+        <v>322.14626700000002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>0.61116899999999996</v>
+      </c>
+      <c r="H5">
+        <v>0.77229999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>12.098867</v>
+      </c>
+      <c r="C6">
+        <v>9.8292479999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.498996</v>
+      </c>
+      <c r="F6">
+        <v>0.10288600000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.37675900000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.63790000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the evaluate script
</commit_message>
<xml_diff>
--- a/Evaluation/speedup table.xlsx
+++ b/Evaluation/speedup table.xlsx
@@ -21,16 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>Sequential</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OpenMPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CUDA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -70,7 +66,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0,000011</t>
+    <t>OpenMPI - 2 thread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenMPI - 4 thread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenMPI - 8 thread</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -396,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -409,25 +413,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -452,7 +456,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>9.6142000000000005E-2</v>
@@ -472,7 +476,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0.122294</v>
@@ -495,45 +499,37 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.15035599999999999</v>
+        <v>0.21098</v>
       </c>
       <c r="C5">
-        <v>7.4898999999999993E-2</v>
+        <v>4.8910000000000004E-3</v>
       </c>
       <c r="D5">
-        <v>2.7390000000000001E-3</v>
-      </c>
-      <c r="E5">
-        <v>1.7E-5</v>
+        <v>1.0095E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.178782</v>
       </c>
       <c r="G5">
-        <v>0.199686</v>
+        <v>0.14721899999999999</v>
       </c>
       <c r="H5">
-        <v>0.75407000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>0.21098</v>
-      </c>
-      <c r="C6">
-        <v>4.8910000000000004E-3</v>
-      </c>
-      <c r="D6">
-        <v>1.0095E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.178782</v>
-      </c>
-      <c r="G6">
-        <v>0.14721899999999999</v>
-      </c>
-      <c r="H6">
         <v>0.75946499999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -545,10 +541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -558,25 +554,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -601,7 +597,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2.4280279999999999</v>
@@ -621,7 +617,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -629,45 +625,40 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>17.892775</v>
+        <v>3.6024859999999999</v>
       </c>
       <c r="C5">
-        <v>6.2186599999999999</v>
+        <v>3.1373679999999999</v>
       </c>
       <c r="D5">
-        <v>22.483117</v>
-      </c>
-      <c r="E5">
-        <v>1.1E-5</v>
+        <v>8.6230000000000005E-3</v>
+      </c>
+      <c r="F5">
+        <v>0.113554</v>
+      </c>
+      <c r="G5">
+        <v>0.44085099999999999</v>
       </c>
       <c r="H5">
-        <v>0.95622700000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3.6024859999999999</v>
-      </c>
-      <c r="C6">
-        <v>3.1373679999999999</v>
-      </c>
-      <c r="D6">
-        <v>8.6230000000000005E-3</v>
-      </c>
-      <c r="F6">
-        <v>0.113554</v>
-      </c>
-      <c r="G6">
-        <v>0.44085099999999999</v>
-      </c>
-      <c r="H6">
         <v>0.90499600000000002</v>
       </c>
     </row>
-    <row r="22" ht="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" ht="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -677,35 +668,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -730,7 +721,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>13.650181</v>
@@ -750,7 +741,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -758,45 +749,37 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>203.485626</v>
+        <v>12.098867</v>
       </c>
       <c r="C5">
-        <v>40.328243999999998</v>
+        <v>9.8292479999999998</v>
       </c>
       <c r="D5">
-        <v>322.14626700000002</v>
-      </c>
-      <c r="E5" t="s">
+        <v>0.498996</v>
+      </c>
+      <c r="F5">
+        <v>0.10288600000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.37675900000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.63790000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="G5">
-        <v>0.61116899999999996</v>
-      </c>
-      <c r="H5">
-        <v>0.77229999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>12.098867</v>
-      </c>
-      <c r="C6">
-        <v>9.8292479999999998</v>
-      </c>
-      <c r="D6">
-        <v>0.498996</v>
-      </c>
-      <c r="F6">
-        <v>0.10288600000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.37675900000000001</v>
-      </c>
-      <c r="H6">
-        <v>0.63790000000000002</v>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the result of evaluation table with openmpi version.
</commit_message>
<xml_diff>
--- a/Evaluation/speedup table.xlsx
+++ b/Evaluation/speedup table.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -521,15 +521,69 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7">
+        <v>0.35618899999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.28678700000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.1346999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.168465</v>
+      </c>
+      <c r="G7">
+        <v>0.19752400000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.75872200000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <v>0.59652400000000005</v>
+      </c>
+      <c r="C8">
+        <v>0.50802400000000003</v>
+      </c>
+      <c r="D8">
+        <v>1.5499999999999999E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.33644499999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.19506999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.75894799999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
+      </c>
+      <c r="B9">
+        <v>1.1245419999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.96390100000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.5279999999999999E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.64569699999999997</v>
+      </c>
+      <c r="G9">
+        <v>0.187301</v>
+      </c>
+      <c r="H9">
+        <v>0.76828399999999997</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +598,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -647,15 +701,69 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7">
+        <v>9.257949</v>
+      </c>
+      <c r="C7">
+        <v>4.2429949999999996</v>
+      </c>
+      <c r="D7">
+        <v>9.1942810000000001</v>
+      </c>
+      <c r="E7">
+        <v>2.5517000000000001E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.609846</v>
+      </c>
+      <c r="H7">
+        <v>0.90499600000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <v>5.4509749999999997</v>
+      </c>
+      <c r="C8">
+        <v>2.3885169999999998</v>
+      </c>
+      <c r="D8">
+        <v>5.2544360000000001</v>
+      </c>
+      <c r="E8">
+        <v>9.7092999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.64267200000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.90499600000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
+      </c>
+      <c r="B9">
+        <v>3.2316660000000001</v>
+      </c>
+      <c r="C9">
+        <v>1.4675720000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.709832</v>
+      </c>
+      <c r="E9">
+        <v>1.1174820000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.62708299999999995</v>
+      </c>
+      <c r="H9">
+        <v>0.91732899999999995</v>
       </c>
     </row>
     <row r="21" ht="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -671,7 +779,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -771,15 +879,66 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7">
+        <v>59.094831999999997</v>
+      </c>
+      <c r="C7">
+        <v>38.845353000000003</v>
+      </c>
+      <c r="D7">
+        <v>36.273127000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.32635399999999998</v>
+      </c>
+      <c r="G7">
+        <v>0.61488600000000004</v>
+      </c>
+      <c r="H7">
+        <v>0.60109999999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8">
+        <v>42.116461999999999</v>
+      </c>
+      <c r="C8">
+        <v>20.788727000000002</v>
+      </c>
+      <c r="D8">
+        <v>38.433629000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.64338899999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.60109999999999997</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
+      </c>
+      <c r="B9">
+        <v>44.992384999999999</v>
+      </c>
+      <c r="C9">
+        <v>23.649346000000001</v>
+      </c>
+      <c r="D9">
+        <v>38.272889999999997</v>
+      </c>
+      <c r="E9">
+        <v>13.576266</v>
+      </c>
+      <c r="G9">
+        <v>0.64712599999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.60160000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>